<commit_message>
added staff count to sample data and helipad widget
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>lab_covid_tests</t>
+  </si>
+  <si>
+    <t>staff</t>
   </si>
   <si>
     <t>McLaren Flint</t>
@@ -357,10 +360,13 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>43.0141228745445</v>
@@ -388,11 +394,14 @@
       </c>
       <c r="J2" s="2">
         <v>483.0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>275.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>43.0215227786436</v>
@@ -420,11 +429,14 @@
       </c>
       <c r="J3" s="2">
         <v>527.0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>425.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>42.890276</v>
@@ -452,6 +464,9 @@
       </c>
       <c r="J4" s="2">
         <v>497.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>394.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>